<commit_message>
updated medical record number and tied static results into export
</commit_message>
<xml_diff>
--- a/lib/templates/EH_results_matrix.xlsx
+++ b/lib/templates/EH_results_matrix.xlsx
@@ -4,12 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22624"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="12840" yWindow="2180" windowWidth="30060" windowHeight="20220" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="20640" yWindow="3320" windowWidth="30060" windowHeight="20220" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Proportion" sheetId="1" r:id="rId1"/>
     <sheet name="CV" sheetId="3" r:id="rId2"/>
-    <sheet name="NQF 0495 Strat1" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -21,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="53">
   <si>
     <t>Name</t>
   </si>
@@ -44,99 +43,15 @@
     <t>NQF ID</t>
   </si>
   <si>
-    <t>AMI1, DEN_0142_0164_0639</t>
-  </si>
-  <si>
-    <t>AMI1, NUM_0142_0164_0639</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AMI2, DEN_0163 </t>
-  </si>
-  <si>
-    <t>AMI2, NUM_0163</t>
-  </si>
-  <si>
-    <t>ASTH, NUM_0338</t>
-  </si>
-  <si>
-    <t>NEWB1, DEN_0480_716_1354</t>
-  </si>
-  <si>
-    <t>NEWB1, NUM_0480_716_1354</t>
-  </si>
-  <si>
-    <t>OB, DEN_0469</t>
-  </si>
-  <si>
-    <t>OB, NUM_0469</t>
-  </si>
-  <si>
-    <t>STROKE, DEN_0435_0437_ 0438_ 0439_ 0440_ 0441_0436</t>
-  </si>
-  <si>
-    <t>STROKE, NUM_0435_ 0438_ 0439_ 0440_ 0441_0436</t>
-  </si>
-  <si>
-    <t>VTE1, DEN_0371_0372</t>
-  </si>
-  <si>
-    <t>VTE1, NUM_0371_0372</t>
-  </si>
-  <si>
-    <t>VTE2, DEN_0376_0373_0374_0375</t>
-  </si>
-  <si>
-    <t>VTE2, NUM_0376_0373_0374_0375</t>
-  </si>
-  <si>
-    <t>ASTH, DEN_0338</t>
-  </si>
-  <si>
-    <t>CAP, DEN_0147</t>
-  </si>
-  <si>
-    <t>CAP, NUM_0147</t>
-  </si>
-  <si>
-    <t>SCIP1, DEN_0453_0527_0528</t>
-  </si>
-  <si>
-    <t>SCIP1, NUM_0453_0527_0528</t>
-  </si>
-  <si>
     <t>Totals</t>
   </si>
   <si>
     <t>MSRPOPL</t>
   </si>
   <si>
-    <t>0495</t>
-  </si>
-  <si>
     <t>Median Time</t>
   </si>
   <si>
-    <t>Median Time from ED Arrival to ED Departure for Admitted ED Patients</t>
-  </si>
-  <si>
-    <t>FA8BE62B-09FB-4B01-8CA8-E3CF1F9A16F6</t>
-  </si>
-  <si>
-    <t>F3441A34-7FEA-4DAB-9907-A19885CFF92F</t>
-  </si>
-  <si>
-    <t>STRAT</t>
-  </si>
-  <si>
-    <t>1509C6DA-2465-4571-A6D4-AD634BE49BE6</t>
-  </si>
-  <si>
-    <t>Note</t>
-  </si>
-  <si>
-    <t>AND: "Occurrence A of Encounter, Performed: Emergency Department Visit" &lt;= 1 hour(s) ends before start of "Occurrence A of Encounter, Performed: Encounter Inpatient"</t>
-  </si>
-  <si>
     <t>EXCP</t>
   </si>
   <si>
@@ -144,6 +59,126 @@
   </si>
   <si>
     <t>Subtitle</t>
+  </si>
+  <si>
+    <t>AMI1,NUM_0142_0164_0639</t>
+  </si>
+  <si>
+    <t>649910f4a9da359b17d7c1b012decc17</t>
+  </si>
+  <si>
+    <t>AMI1,DEN_0142_0164_0639</t>
+  </si>
+  <si>
+    <t>caf50e70e548d61d097c68e9001ded60</t>
+  </si>
+  <si>
+    <t>AMI2,DEN_0163</t>
+  </si>
+  <si>
+    <t>b03719c7f99502b7990918baf4640f70</t>
+  </si>
+  <si>
+    <t>AMI2,NUM_0163</t>
+  </si>
+  <si>
+    <t>116c5a883ccdc89b2531bcbae3a403ab</t>
+  </si>
+  <si>
+    <t>ASTH,DEN_0338</t>
+  </si>
+  <si>
+    <t>4a2c0f51c82d7f481ed992047f377cb9</t>
+  </si>
+  <si>
+    <t>ASTH,NUM_0338</t>
+  </si>
+  <si>
+    <t>29778d9cb06701de524b752c1f4de992</t>
+  </si>
+  <si>
+    <t>CAP,DEN_0147</t>
+  </si>
+  <si>
+    <t>8f0d70dbd636c1ab0fac0552ea9ec459</t>
+  </si>
+  <si>
+    <t>CAP,NUM_0147</t>
+  </si>
+  <si>
+    <t>26ed1a80db1e5d2515a738290af8a47f</t>
+  </si>
+  <si>
+    <t>NEWB,DEN_0480_0716_1354</t>
+  </si>
+  <si>
+    <t>1ef57c0a5ac2ef5a2b50b3f4bb04d76c</t>
+  </si>
+  <si>
+    <t>NEWB,NUM_0480_0716_1354</t>
+  </si>
+  <si>
+    <t>f03f9bf5cc4bfa7298ae1a4804cc7e5f</t>
+  </si>
+  <si>
+    <t>OB,DEN_0469</t>
+  </si>
+  <si>
+    <t>c9793858086073dd8469711347526120</t>
+  </si>
+  <si>
+    <t>OB,NUM_0469</t>
+  </si>
+  <si>
+    <t>e46ad0c62f53106c5b190ef7b074bd6d</t>
+  </si>
+  <si>
+    <t>SCIP,DEN_0453_0527_0528</t>
+  </si>
+  <si>
+    <t>4419c3df96d1e9699136eaa29b9cd44b</t>
+  </si>
+  <si>
+    <t>SCIP,NUM_0453_0527_0528</t>
+  </si>
+  <si>
+    <t>1d498bdc11d16adefd411599c04be5ee</t>
+  </si>
+  <si>
+    <t>STROKE,DEN_0435_0436_0437_ 0438_ 0439_ 0440_ 0441</t>
+  </si>
+  <si>
+    <t>879223b7a0d9fee24b76afac7e1ce268</t>
+  </si>
+  <si>
+    <t>STROKE,NUM_0435_0436_0437_0438_ 0439_ 0440_ 0441</t>
+  </si>
+  <si>
+    <t>8f9b441a0e9f8c63a55bd282d864671c</t>
+  </si>
+  <si>
+    <t>VTE1,NUM_0371_0372</t>
+  </si>
+  <si>
+    <t>b1a31a5c5207d1fb0767076f87ce3870</t>
+  </si>
+  <si>
+    <t>VTE1,DEN_0371_0372</t>
+  </si>
+  <si>
+    <t>daf670caaec4a8c386a5ccea3b64e0a5</t>
+  </si>
+  <si>
+    <t>VTE2,DEN_0373_0374_0375_0376</t>
+  </si>
+  <si>
+    <t>331280e8aaa30dd1526842ef98498b49</t>
+  </si>
+  <si>
+    <t>VTE2,NUM_0373_0374_0375_0376</t>
+  </si>
+  <si>
+    <t>312f7d09e90ed9ca35617715178893fd</t>
   </si>
 </sst>
 </file>
@@ -230,16 +265,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="23">
@@ -267,17 +299,7 @@
     <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -628,13 +650,13 @@
   <dimension ref="A1:I23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="49.5" customWidth="1"/>
-    <col min="2" max="2" width="24" style="1" customWidth="1"/>
+    <col min="2" max="2" width="33.5" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="38.33203125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -658,15 +680,15 @@
         <v>5</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>38</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="2">
-        <v>4.2602048200914801E+18</v>
+        <v>13</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>14</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
@@ -679,10 +701,10 @@
     </row>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="2">
-        <v>3.7027422446020602E+17</v>
+        <v>15</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>16</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
@@ -695,10 +717,10 @@
     </row>
     <row r="4" spans="1:8">
       <c r="A4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="2">
-        <v>7.1881498866333798E+17</v>
+        <v>17</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>18</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
@@ -706,15 +728,15 @@
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
       <c r="H4" s="4" t="s">
-        <v>40</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" s="2">
-        <v>1.44333622242925E+18</v>
+        <v>19</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>20</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
@@ -727,10 +749,10 @@
     </row>
     <row r="6" spans="1:8">
       <c r="A6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>22</v>
-      </c>
-      <c r="B6" s="2">
-        <v>4.5673965903119201E+18</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
@@ -743,10 +765,10 @@
     </row>
     <row r="7" spans="1:8">
       <c r="A7" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" s="2">
-        <v>2.5161863788008202E+18</v>
+        <v>23</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>24</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
@@ -759,10 +781,10 @@
     </row>
     <row r="8" spans="1:8">
       <c r="A8" t="s">
-        <v>23</v>
-      </c>
-      <c r="B8" s="2">
-        <v>7.3927701307493798E+17</v>
+        <v>25</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>26</v>
       </c>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
@@ -775,10 +797,10 @@
     </row>
     <row r="9" spans="1:8">
       <c r="A9" t="s">
-        <v>24</v>
-      </c>
-      <c r="B9" s="2">
-        <v>1.7842405250990899E+18</v>
+        <v>27</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>28</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
@@ -789,10 +811,10 @@
     </row>
     <row r="10" spans="1:8">
       <c r="A10" t="s">
-        <v>12</v>
-      </c>
-      <c r="B10" s="2">
-        <v>2.5870571370871699E+17</v>
+        <v>29</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>30</v>
       </c>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
@@ -803,10 +825,10 @@
     </row>
     <row r="11" spans="1:8">
       <c r="A11" t="s">
-        <v>13</v>
-      </c>
-      <c r="B11" s="2">
-        <v>4.4398635657095598E+18</v>
+        <v>31</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>32</v>
       </c>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
@@ -817,10 +839,10 @@
     </row>
     <row r="12" spans="1:8">
       <c r="A12" t="s">
-        <v>14</v>
-      </c>
-      <c r="B12" s="2">
-        <v>3.0019447262852598E+18</v>
+        <v>33</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>34</v>
       </c>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
@@ -831,10 +853,10 @@
     </row>
     <row r="13" spans="1:8">
       <c r="A13" t="s">
-        <v>15</v>
-      </c>
-      <c r="B13" s="2">
-        <v>9.20351064105248E+17</v>
+        <v>35</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>36</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
@@ -845,10 +867,10 @@
     </row>
     <row r="14" spans="1:8">
       <c r="A14" t="s">
-        <v>25</v>
-      </c>
-      <c r="B14" s="2">
-        <v>1.47638719185794E+18</v>
+        <v>37</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
@@ -859,10 +881,10 @@
     </row>
     <row r="15" spans="1:8">
       <c r="A15" t="s">
-        <v>26</v>
-      </c>
-      <c r="B15" s="2">
-        <v>3.66738262042242E+18</v>
+        <v>39</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>40</v>
       </c>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
@@ -873,10 +895,10 @@
     </row>
     <row r="16" spans="1:8">
       <c r="A16" t="s">
-        <v>16</v>
-      </c>
-      <c r="B16" s="2">
-        <v>3.6254654017590702E+18</v>
+        <v>41</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>42</v>
       </c>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
@@ -887,10 +909,10 @@
     </row>
     <row r="17" spans="1:8">
       <c r="A17" t="s">
-        <v>17</v>
-      </c>
-      <c r="B17" s="2">
-        <v>5.5056563459271098E+17</v>
+        <v>43</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>44</v>
       </c>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
@@ -901,10 +923,10 @@
     </row>
     <row r="18" spans="1:8">
       <c r="A18" t="s">
-        <v>18</v>
-      </c>
-      <c r="B18" s="2">
-        <v>1.2980835496957599E+18</v>
+        <v>45</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>46</v>
       </c>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
@@ -915,10 +937,10 @@
     </row>
     <row r="19" spans="1:8">
       <c r="A19" t="s">
-        <v>19</v>
-      </c>
-      <c r="B19" s="2">
-        <v>3.9691425105378202E+18</v>
+        <v>47</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>48</v>
       </c>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
@@ -929,10 +951,10 @@
     </row>
     <row r="20" spans="1:8">
       <c r="A20" t="s">
-        <v>20</v>
-      </c>
-      <c r="B20" s="2">
-        <v>4.4191854368146698E+18</v>
+        <v>49</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>50</v>
       </c>
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
@@ -943,10 +965,10 @@
     </row>
     <row r="21" spans="1:8">
       <c r="A21" t="s">
-        <v>21</v>
-      </c>
-      <c r="B21" s="2">
-        <v>1.5890344101935601E+18</v>
+        <v>51</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>52</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
@@ -965,32 +987,32 @@
     </row>
     <row r="23" spans="1:8">
       <c r="B23" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C23">
-        <f>COUNTA(C2:C21)</f>
+        <v>7</v>
+      </c>
+      <c r="C23" s="2">
+        <f>SUM(C2:C21)</f>
         <v>0</v>
       </c>
-      <c r="D23">
-        <f t="shared" ref="D23:G23" si="0">COUNTA(D2:D21)</f>
+      <c r="D23" s="2">
+        <f t="shared" ref="D23:G23" si="0">SUM(D2:D21)</f>
         <v>0</v>
       </c>
-      <c r="E23">
+      <c r="E23" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F23">
+      <c r="F23" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G23">
+      <c r="G23" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="C2:G21">
-    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",C2)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1009,13 +1031,13 @@
   <dimension ref="A1:I23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="49.5" customWidth="1"/>
-    <col min="2" max="2" width="24" style="1" customWidth="1"/>
+    <col min="2" max="2" width="33.5" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.33203125" customWidth="1"/>
     <col min="9" max="9" width="38.33203125" style="1" customWidth="1"/>
   </cols>
@@ -1031,16 +1053,16 @@
         <v>2</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>28</v>
+        <v>8</v>
       </c>
       <c r="F1" s="4"/>
     </row>
     <row r="2" spans="1:9">
       <c r="A2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="2">
-        <v>4.2602048200914801E+18</v>
+        <v>13</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>14</v>
       </c>
       <c r="H2" s="4" t="s">
         <v>0</v>
@@ -1049,32 +1071,32 @@
     </row>
     <row r="3" spans="1:9">
       <c r="A3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="2">
-        <v>3.7027422446020602E+17</v>
+        <v>15</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>16</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>40</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:9">
       <c r="A4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="2">
-        <v>7.1881498866333798E+17</v>
+        <v>17</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>18</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:9">
       <c r="A5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" s="2">
-        <v>1.44333622242925E+18</v>
+        <v>19</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>20</v>
       </c>
       <c r="H5" s="4" t="s">
         <v>2</v>
@@ -1082,181 +1104,181 @@
     </row>
     <row r="6" spans="1:9">
       <c r="A6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B6" s="2">
-        <v>4.5673965903119201E+18</v>
-      </c>
       <c r="H6" s="4" t="s">
-        <v>28</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:9">
       <c r="A7" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" s="2">
-        <v>2.5161863788008202E+18</v>
+        <v>23</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>24</v>
       </c>
       <c r="H7" s="4"/>
-      <c r="I7" s="7"/>
+      <c r="I7" s="6"/>
     </row>
     <row r="8" spans="1:9">
       <c r="A8" t="s">
-        <v>23</v>
-      </c>
-      <c r="B8" s="2">
-        <v>7.3927701307493798E+17</v>
+        <v>25</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>26</v>
       </c>
       <c r="H8" s="4"/>
-      <c r="I8" s="7" t="s">
-        <v>39</v>
+      <c r="I8" s="6" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:9">
       <c r="A9" t="s">
-        <v>24</v>
-      </c>
-      <c r="B9" s="2">
-        <v>1.7842405250990899E+18</v>
+        <v>27</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>28</v>
       </c>
       <c r="H9" s="4"/>
-      <c r="I9" s="7"/>
+      <c r="I9" s="6"/>
     </row>
     <row r="10" spans="1:9">
       <c r="A10" t="s">
-        <v>12</v>
-      </c>
-      <c r="B10" s="2">
-        <v>2.5870571370871699E+17</v>
+        <v>29</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>30</v>
       </c>
       <c r="H10" s="4"/>
-      <c r="I10" s="7"/>
+      <c r="I10" s="6"/>
     </row>
     <row r="11" spans="1:9">
       <c r="A11" t="s">
-        <v>13</v>
-      </c>
-      <c r="B11" s="2">
-        <v>4.4398635657095598E+18</v>
+        <v>31</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>32</v>
       </c>
       <c r="H11" s="4"/>
-      <c r="I11" s="7"/>
+      <c r="I11" s="6"/>
     </row>
     <row r="12" spans="1:9">
       <c r="A12" t="s">
-        <v>14</v>
-      </c>
-      <c r="B12" s="2">
-        <v>3.0019447262852598E+18</v>
+        <v>33</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>34</v>
       </c>
       <c r="H12" s="4"/>
-      <c r="I12" s="7"/>
+      <c r="I12" s="6"/>
     </row>
     <row r="13" spans="1:9">
       <c r="A13" t="s">
-        <v>15</v>
-      </c>
-      <c r="B13" s="2">
-        <v>9.20351064105248E+17</v>
+        <v>35</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>36</v>
       </c>
       <c r="H13" s="4"/>
-      <c r="I13" s="7"/>
+      <c r="I13" s="6"/>
     </row>
     <row r="14" spans="1:9">
       <c r="A14" t="s">
-        <v>25</v>
-      </c>
-      <c r="B14" s="2">
-        <v>1.47638719185794E+18</v>
+        <v>37</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="H14" s="4"/>
-      <c r="I14" s="7"/>
+      <c r="I14" s="6"/>
     </row>
     <row r="15" spans="1:9">
       <c r="A15" t="s">
-        <v>26</v>
-      </c>
-      <c r="B15" s="2">
-        <v>3.66738262042242E+18</v>
+        <v>39</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>40</v>
       </c>
       <c r="H15" s="4"/>
-      <c r="I15" s="7"/>
+      <c r="I15" s="6"/>
     </row>
     <row r="16" spans="1:9">
       <c r="A16" t="s">
-        <v>16</v>
-      </c>
-      <c r="B16" s="2">
-        <v>3.6254654017590702E+18</v>
+        <v>41</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>42</v>
       </c>
       <c r="H16" s="4"/>
-      <c r="I16" s="7"/>
+      <c r="I16" s="6"/>
     </row>
     <row r="17" spans="1:9">
       <c r="A17" t="s">
-        <v>17</v>
-      </c>
-      <c r="B17" s="2">
-        <v>5.5056563459271098E+17</v>
+        <v>43</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>44</v>
       </c>
       <c r="H17" s="4"/>
-      <c r="I17" s="7"/>
+      <c r="I17" s="6"/>
     </row>
     <row r="18" spans="1:9">
       <c r="A18" t="s">
-        <v>18</v>
-      </c>
-      <c r="B18" s="2">
-        <v>1.2980835496957599E+18</v>
+        <v>45</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>46</v>
       </c>
       <c r="H18" s="4"/>
-      <c r="I18" s="7"/>
+      <c r="I18" s="6"/>
     </row>
     <row r="19" spans="1:9">
       <c r="A19" t="s">
-        <v>19</v>
-      </c>
-      <c r="B19" s="2">
-        <v>3.9691425105378202E+18</v>
+        <v>47</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>48</v>
       </c>
       <c r="H19" s="4"/>
-      <c r="I19" s="7"/>
+      <c r="I19" s="6"/>
     </row>
     <row r="20" spans="1:9">
       <c r="A20" t="s">
-        <v>20</v>
-      </c>
-      <c r="B20" s="2">
-        <v>4.4191854368146698E+18</v>
+        <v>49</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>50</v>
       </c>
       <c r="H20" s="4"/>
-      <c r="I20" s="7"/>
+      <c r="I20" s="6"/>
     </row>
     <row r="21" spans="1:9">
       <c r="A21" t="s">
-        <v>21</v>
-      </c>
-      <c r="B21" s="2">
-        <v>1.5890344101935601E+18</v>
+        <v>51</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>52</v>
       </c>
       <c r="H21" s="4"/>
-      <c r="I21" s="7"/>
+      <c r="I21" s="6"/>
     </row>
     <row r="22" spans="1:9">
       <c r="H22" s="4"/>
-      <c r="I22" s="7"/>
+      <c r="I22" s="6"/>
     </row>
     <row r="23" spans="1:9">
       <c r="B23" s="3" t="s">
-        <v>27</v>
+        <v>7</v>
       </c>
       <c r="C23">
-        <f>COUNTA(C2:C21)</f>
+        <f>SUM(C2:C21)</f>
         <v>0</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>30</v>
+        <v>9</v>
       </c>
       <c r="E23" t="e">
         <f>MEDIAN(E2:E21)</f>
@@ -1264,338 +1286,6 @@
       </c>
       <c r="H23" s="4"/>
       <c r="I23" s="3"/>
-    </row>
-  </sheetData>
-  <conditionalFormatting sqref="C2:C21 E2:G21">
-    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="TRUE">
-      <formula>NOT(ISERROR(SEARCH("TRUE",C2)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I23"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6:E7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
-  <cols>
-    <col min="1" max="1" width="49.5" customWidth="1"/>
-    <col min="2" max="2" width="24" style="1" customWidth="1"/>
-    <col min="4" max="4" width="12.33203125" customWidth="1"/>
-    <col min="9" max="9" width="38.33203125" style="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9">
-      <c r="A1" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="F1" s="4"/>
-    </row>
-    <row r="2" spans="1:9">
-      <c r="A2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="2">
-        <v>4.2602048200914801E+18</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="E2">
-        <v>50</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="I2" s="5" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9">
-      <c r="A3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="2">
-        <v>3.7027422446020602E+17</v>
-      </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="E3">
-        <v>50</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9">
-      <c r="A4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="2">
-        <v>7.1881498866333798E+17</v>
-      </c>
-      <c r="C4">
-        <v>1</v>
-      </c>
-      <c r="E4">
-        <v>50</v>
-      </c>
-      <c r="H4" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9">
-      <c r="A5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" s="2">
-        <v>1.44333622242925E+18</v>
-      </c>
-      <c r="C5">
-        <v>1</v>
-      </c>
-      <c r="E5">
-        <v>50</v>
-      </c>
-      <c r="H5" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9">
-      <c r="A6" t="s">
-        <v>22</v>
-      </c>
-      <c r="B6" s="2">
-        <v>4.5673965903119201E+18</v>
-      </c>
-      <c r="H6" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9">
-      <c r="A7" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" s="2">
-        <v>2.5161863788008202E+18</v>
-      </c>
-      <c r="H7" s="4"/>
-    </row>
-    <row r="8" spans="1:9">
-      <c r="A8" t="s">
-        <v>23</v>
-      </c>
-      <c r="B8" s="2">
-        <v>7.3927701307493798E+17</v>
-      </c>
-      <c r="C8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9">
-      <c r="A9" t="s">
-        <v>24</v>
-      </c>
-      <c r="B9" s="2">
-        <v>1.7842405250990899E+18</v>
-      </c>
-      <c r="C9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9">
-      <c r="A10" t="s">
-        <v>12</v>
-      </c>
-      <c r="B10" s="2">
-        <v>2.5870571370871699E+17</v>
-      </c>
-      <c r="C10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9">
-      <c r="A11" t="s">
-        <v>13</v>
-      </c>
-      <c r="B11" s="2">
-        <v>4.4398635657095598E+18</v>
-      </c>
-      <c r="C11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9">
-      <c r="A12" t="s">
-        <v>14</v>
-      </c>
-      <c r="B12" s="2">
-        <v>3.0019447262852598E+18</v>
-      </c>
-      <c r="C12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9">
-      <c r="A13" t="s">
-        <v>15</v>
-      </c>
-      <c r="B13" s="2">
-        <v>9.20351064105248E+17</v>
-      </c>
-      <c r="C13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9">
-      <c r="A14" t="s">
-        <v>25</v>
-      </c>
-      <c r="B14" s="2">
-        <v>1.47638719185794E+18</v>
-      </c>
-      <c r="C14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9">
-      <c r="A15" t="s">
-        <v>26</v>
-      </c>
-      <c r="B15" s="2">
-        <v>3.66738262042242E+18</v>
-      </c>
-      <c r="C15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9">
-      <c r="A16" t="s">
-        <v>16</v>
-      </c>
-      <c r="B16" s="2">
-        <v>3.6254654017590702E+18</v>
-      </c>
-      <c r="C16">
-        <v>1</v>
-      </c>
-      <c r="E16">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9">
-      <c r="A17" t="s">
-        <v>17</v>
-      </c>
-      <c r="B17" s="2">
-        <v>5.5056563459271098E+17</v>
-      </c>
-      <c r="C17">
-        <v>1</v>
-      </c>
-      <c r="E17">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9">
-      <c r="A18" t="s">
-        <v>18</v>
-      </c>
-      <c r="B18" s="2">
-        <v>1.2980835496957599E+18</v>
-      </c>
-      <c r="C18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9">
-      <c r="A19" t="s">
-        <v>19</v>
-      </c>
-      <c r="B19" s="2">
-        <v>3.9691425105378202E+18</v>
-      </c>
-      <c r="C19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9">
-      <c r="A20" t="s">
-        <v>20</v>
-      </c>
-      <c r="B20" s="2">
-        <v>4.4191854368146698E+18</v>
-      </c>
-      <c r="C20">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9">
-      <c r="A21" t="s">
-        <v>21</v>
-      </c>
-      <c r="B21" s="2">
-        <v>1.5890344101935601E+18</v>
-      </c>
-      <c r="C21">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" ht="71">
-      <c r="B23" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C23">
-        <f>COUNTA(C2:C21)</f>
-        <v>18</v>
-      </c>
-      <c r="D23" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="E23">
-        <f>MEDIAN(E2:E21)</f>
-        <v>50</v>
-      </c>
-      <c r="H23" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="I23" s="6" t="s">
-        <v>37</v>
-      </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="C2:C21 E2:G21">

</xml_diff>

<commit_message>
updated patients listed in EH static template
</commit_message>
<xml_diff>
--- a/lib/templates/EH_results_matrix.xlsx
+++ b/lib/templates/EH_results_matrix.xlsx
@@ -85,30 +85,12 @@
     <t>116c5a883ccdc89b2531bcbae3a403ab</t>
   </si>
   <si>
-    <t>ASTH,DEN_0338</t>
-  </si>
-  <si>
-    <t>4a2c0f51c82d7f481ed992047f377cb9</t>
-  </si>
-  <si>
     <t>ASTH,NUM_0338</t>
   </si>
   <si>
     <t>29778d9cb06701de524b752c1f4de992</t>
   </si>
   <si>
-    <t>CAP,DEN_0147</t>
-  </si>
-  <si>
-    <t>8f0d70dbd636c1ab0fac0552ea9ec459</t>
-  </si>
-  <si>
-    <t>CAP,NUM_0147</t>
-  </si>
-  <si>
-    <t>26ed1a80db1e5d2515a738290af8a47f</t>
-  </si>
-  <si>
     <t>NEWB,DEN_0480_0716_1354</t>
   </si>
   <si>
@@ -121,18 +103,6 @@
     <t>f03f9bf5cc4bfa7298ae1a4804cc7e5f</t>
   </si>
   <si>
-    <t>OB,DEN_0469</t>
-  </si>
-  <si>
-    <t>c9793858086073dd8469711347526120</t>
-  </si>
-  <si>
-    <t>OB,NUM_0469</t>
-  </si>
-  <si>
-    <t>e46ad0c62f53106c5b190ef7b074bd6d</t>
-  </si>
-  <si>
     <t>SCIP,DEN_0453_0527_0528</t>
   </si>
   <si>
@@ -151,34 +121,64 @@
     <t>879223b7a0d9fee24b76afac7e1ce268</t>
   </si>
   <si>
-    <t>STROKE,NUM_0435_0436_0437_0438_ 0439_ 0440_ 0441</t>
-  </si>
-  <si>
-    <t>8f9b441a0e9f8c63a55bd282d864671c</t>
-  </si>
-  <si>
-    <t>VTE1,NUM_0371_0372</t>
-  </si>
-  <si>
-    <t>b1a31a5c5207d1fb0767076f87ce3870</t>
-  </si>
-  <si>
-    <t>VTE1,DEN_0371_0372</t>
-  </si>
-  <si>
-    <t>daf670caaec4a8c386a5ccea3b64e0a5</t>
-  </si>
-  <si>
-    <t>VTE2,DEN_0373_0374_0375_0376</t>
-  </si>
-  <si>
-    <t>331280e8aaa30dd1526842ef98498b49</t>
-  </si>
-  <si>
-    <t>VTE2,NUM_0373_0374_0375_0376</t>
-  </si>
-  <si>
-    <t>312f7d09e90ed9ca35617715178893fd</t>
+    <t>ASTH,DEN_0338_496</t>
+  </si>
+  <si>
+    <t>3f3a63ed0f7c69e7d39e0f7f6f123151</t>
+  </si>
+  <si>
+    <t>CAP,DEN_0147_372</t>
+  </si>
+  <si>
+    <t>4f2694161da81fb6d16f6fb421239e3d</t>
+  </si>
+  <si>
+    <t>CAP,NUM_0147_372</t>
+  </si>
+  <si>
+    <t>e9f710b1f129c10bf69d3c29432e166f</t>
+  </si>
+  <si>
+    <t>OB,DEN_0469_376</t>
+  </si>
+  <si>
+    <t>52e4994176da107bf82584a316146e68</t>
+  </si>
+  <si>
+    <t>OB,NUM_0469_0376</t>
+  </si>
+  <si>
+    <t>f8745b14e07f41c49d8785a1d9920b77</t>
+  </si>
+  <si>
+    <t>STROKE,NUM_0435_0436_0437_ 0439_ 0440_ 0441</t>
+  </si>
+  <si>
+    <t>e8932b4783869759f5217d12cc6efd19</t>
+  </si>
+  <si>
+    <t>STROKE,NUM_ 0438</t>
+  </si>
+  <si>
+    <t>cce692bcfd3d4dc602a052190bb30d8b</t>
+  </si>
+  <si>
+    <t>VTE1,NUM_0371</t>
+  </si>
+  <si>
+    <t>59074d1606548365d4db75931397082c</t>
+  </si>
+  <si>
+    <t>VTE2,DEN_0373_0374_0375</t>
+  </si>
+  <si>
+    <t>c6bbb7342c4cf4ebeeaf1a417646db69</t>
+  </si>
+  <si>
+    <t>VTE2,NUM_0373_0374_0375</t>
+  </si>
+  <si>
+    <t>6d4da8955b5aee38deb098909d3c4a06</t>
   </si>
 </sst>
 </file>
@@ -240,8 +240,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="23">
+  <cellStyleXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -274,7 +276,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="23">
+  <cellStyles count="25">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -286,6 +288,7 @@
     <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -297,6 +300,7 @@
     <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="2">
@@ -650,7 +654,7 @@
   <dimension ref="A1:I23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="A2" sqref="A2:B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -684,11 +688,11 @@
       </c>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" t="s">
-        <v>13</v>
+      <c r="A2" s="2" t="s">
+        <v>15</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
@@ -700,11 +704,11 @@
       </c>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" t="s">
-        <v>15</v>
+      <c r="A3" s="2" t="s">
+        <v>13</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
@@ -716,7 +720,7 @@
       </c>
     </row>
     <row r="4" spans="1:8">
-      <c r="A4" t="s">
+      <c r="A4" s="2" t="s">
         <v>17</v>
       </c>
       <c r="B4" s="2" t="s">
@@ -732,7 +736,7 @@
       </c>
     </row>
     <row r="5" spans="1:8">
-      <c r="A5" t="s">
+      <c r="A5" s="2" t="s">
         <v>19</v>
       </c>
       <c r="B5" s="2" t="s">
@@ -748,11 +752,11 @@
       </c>
     </row>
     <row r="6" spans="1:8">
-      <c r="A6" t="s">
-        <v>21</v>
+      <c r="A6" s="2" t="s">
+        <v>33</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
@@ -764,11 +768,11 @@
       </c>
     </row>
     <row r="7" spans="1:8">
-      <c r="A7" t="s">
-        <v>23</v>
+      <c r="A7" s="2" t="s">
+        <v>21</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
@@ -780,11 +784,11 @@
       </c>
     </row>
     <row r="8" spans="1:8">
-      <c r="A8" t="s">
-        <v>25</v>
+      <c r="A8" s="2" t="s">
+        <v>35</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
@@ -796,11 +800,11 @@
       </c>
     </row>
     <row r="9" spans="1:8">
-      <c r="A9" t="s">
-        <v>27</v>
+      <c r="A9" s="2" t="s">
+        <v>37</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
@@ -810,11 +814,11 @@
       <c r="H9" s="4"/>
     </row>
     <row r="10" spans="1:8">
-      <c r="A10" t="s">
-        <v>29</v>
+      <c r="A10" s="2" t="s">
+        <v>23</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
@@ -824,11 +828,11 @@
       <c r="H10" s="4"/>
     </row>
     <row r="11" spans="1:8">
-      <c r="A11" t="s">
-        <v>31</v>
+      <c r="A11" s="2" t="s">
+        <v>25</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
@@ -838,11 +842,11 @@
       <c r="H11" s="4"/>
     </row>
     <row r="12" spans="1:8">
-      <c r="A12" t="s">
-        <v>33</v>
+      <c r="A12" s="2" t="s">
+        <v>39</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
@@ -852,11 +856,11 @@
       <c r="H12" s="4"/>
     </row>
     <row r="13" spans="1:8">
-      <c r="A13" t="s">
-        <v>35</v>
+      <c r="A13" s="2" t="s">
+        <v>41</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
@@ -866,11 +870,11 @@
       <c r="H13" s="4"/>
     </row>
     <row r="14" spans="1:8">
-      <c r="A14" t="s">
-        <v>37</v>
+      <c r="A14" s="2" t="s">
+        <v>27</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
@@ -880,11 +884,11 @@
       <c r="H14" s="4"/>
     </row>
     <row r="15" spans="1:8">
-      <c r="A15" t="s">
-        <v>39</v>
+      <c r="A15" s="2" t="s">
+        <v>29</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
@@ -894,11 +898,11 @@
       <c r="H15" s="4"/>
     </row>
     <row r="16" spans="1:8">
-      <c r="A16" t="s">
-        <v>41</v>
+      <c r="A16" s="2" t="s">
+        <v>31</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
@@ -908,7 +912,7 @@
       <c r="H16" s="4"/>
     </row>
     <row r="17" spans="1:8">
-      <c r="A17" t="s">
+      <c r="A17" s="2" t="s">
         <v>43</v>
       </c>
       <c r="B17" s="2" t="s">
@@ -922,7 +926,7 @@
       <c r="H17" s="4"/>
     </row>
     <row r="18" spans="1:8">
-      <c r="A18" t="s">
+      <c r="A18" s="2" t="s">
         <v>45</v>
       </c>
       <c r="B18" s="2" t="s">
@@ -936,7 +940,7 @@
       <c r="H18" s="4"/>
     </row>
     <row r="19" spans="1:8">
-      <c r="A19" t="s">
+      <c r="A19" s="2" t="s">
         <v>47</v>
       </c>
       <c r="B19" s="2" t="s">
@@ -950,7 +954,7 @@
       <c r="H19" s="4"/>
     </row>
     <row r="20" spans="1:8">
-      <c r="A20" t="s">
+      <c r="A20" s="2" t="s">
         <v>49</v>
       </c>
       <c r="B20" s="2" t="s">
@@ -964,7 +968,7 @@
       <c r="H20" s="4"/>
     </row>
     <row r="21" spans="1:8">
-      <c r="A21" t="s">
+      <c r="A21" s="2" t="s">
         <v>51</v>
       </c>
       <c r="B21" s="2" t="s">
@@ -1031,7 +1035,7 @@
   <dimension ref="A1:I23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+      <selection activeCell="A2" sqref="A2:B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1058,11 +1062,11 @@
       <c r="F1" s="4"/>
     </row>
     <row r="2" spans="1:9">
-      <c r="A2" t="s">
-        <v>13</v>
+      <c r="A2" s="2" t="s">
+        <v>15</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="H2" s="4" t="s">
         <v>0</v>
@@ -1070,18 +1074,18 @@
       <c r="I2" s="5"/>
     </row>
     <row r="3" spans="1:9">
-      <c r="A3" t="s">
-        <v>15</v>
+      <c r="A3" s="2" t="s">
+        <v>13</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="H3" s="4" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:9">
-      <c r="A4" t="s">
+      <c r="A4" s="2" t="s">
         <v>17</v>
       </c>
       <c r="B4" s="2" t="s">
@@ -1092,7 +1096,7 @@
       </c>
     </row>
     <row r="5" spans="1:9">
-      <c r="A5" t="s">
+      <c r="A5" s="2" t="s">
         <v>19</v>
       </c>
       <c r="B5" s="2" t="s">
@@ -1103,32 +1107,32 @@
       </c>
     </row>
     <row r="6" spans="1:9">
-      <c r="A6" t="s">
-        <v>21</v>
+      <c r="A6" s="2" t="s">
+        <v>33</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="H6" s="4" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:9">
-      <c r="A7" t="s">
-        <v>23</v>
+      <c r="A7" s="2" t="s">
+        <v>21</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="H7" s="4"/>
       <c r="I7" s="6"/>
     </row>
     <row r="8" spans="1:9">
-      <c r="A8" t="s">
-        <v>25</v>
+      <c r="A8" s="2" t="s">
+        <v>35</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="H8" s="4"/>
       <c r="I8" s="6" t="s">
@@ -1136,87 +1140,87 @@
       </c>
     </row>
     <row r="9" spans="1:9">
-      <c r="A9" t="s">
-        <v>27</v>
+      <c r="A9" s="2" t="s">
+        <v>37</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="H9" s="4"/>
       <c r="I9" s="6"/>
     </row>
     <row r="10" spans="1:9">
-      <c r="A10" t="s">
-        <v>29</v>
+      <c r="A10" s="2" t="s">
+        <v>23</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="H10" s="4"/>
       <c r="I10" s="6"/>
     </row>
     <row r="11" spans="1:9">
-      <c r="A11" t="s">
-        <v>31</v>
+      <c r="A11" s="2" t="s">
+        <v>25</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="H11" s="4"/>
       <c r="I11" s="6"/>
     </row>
     <row r="12" spans="1:9">
-      <c r="A12" t="s">
-        <v>33</v>
+      <c r="A12" s="2" t="s">
+        <v>39</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="H12" s="4"/>
       <c r="I12" s="6"/>
     </row>
     <row r="13" spans="1:9">
-      <c r="A13" t="s">
-        <v>35</v>
+      <c r="A13" s="2" t="s">
+        <v>41</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="H13" s="4"/>
       <c r="I13" s="6"/>
     </row>
     <row r="14" spans="1:9">
-      <c r="A14" t="s">
-        <v>37</v>
+      <c r="A14" s="2" t="s">
+        <v>27</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="H14" s="4"/>
       <c r="I14" s="6"/>
     </row>
     <row r="15" spans="1:9">
-      <c r="A15" t="s">
-        <v>39</v>
+      <c r="A15" s="2" t="s">
+        <v>29</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="H15" s="4"/>
       <c r="I15" s="6"/>
     </row>
     <row r="16" spans="1:9">
-      <c r="A16" t="s">
-        <v>41</v>
+      <c r="A16" s="2" t="s">
+        <v>31</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="H16" s="4"/>
       <c r="I16" s="6"/>
     </row>
     <row r="17" spans="1:9">
-      <c r="A17" t="s">
+      <c r="A17" s="2" t="s">
         <v>43</v>
       </c>
       <c r="B17" s="2" t="s">
@@ -1226,7 +1230,7 @@
       <c r="I17" s="6"/>
     </row>
     <row r="18" spans="1:9">
-      <c r="A18" t="s">
+      <c r="A18" s="2" t="s">
         <v>45</v>
       </c>
       <c r="B18" s="2" t="s">
@@ -1236,7 +1240,7 @@
       <c r="I18" s="6"/>
     </row>
     <row r="19" spans="1:9">
-      <c r="A19" t="s">
+      <c r="A19" s="2" t="s">
         <v>47</v>
       </c>
       <c r="B19" s="2" t="s">
@@ -1246,7 +1250,7 @@
       <c r="I19" s="6"/>
     </row>
     <row r="20" spans="1:9">
-      <c r="A20" t="s">
+      <c r="A20" s="2" t="s">
         <v>49</v>
       </c>
       <c r="B20" s="2" t="s">
@@ -1256,7 +1260,7 @@
       <c r="I20" s="6"/>
     </row>
     <row r="21" spans="1:9">
-      <c r="A21" t="s">
+      <c r="A21" s="2" t="s">
         <v>51</v>
       </c>
       <c r="B21" s="2" t="s">

</xml_diff>

<commit_message>
added measure observation logic for CV measures
</commit_message>
<xml_diff>
--- a/lib/templates/EH_results_matrix.xlsx
+++ b/lib/templates/EH_results_matrix.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22624"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="20640" yWindow="3320" windowWidth="30060" windowHeight="20220" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="7960" yWindow="2020" windowWidth="30060" windowHeight="20220" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Proportion" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="54">
   <si>
     <t>Name</t>
   </si>
@@ -179,6 +179,9 @@
   </si>
   <si>
     <t>6d4da8955b5aee38deb098909d3c4a06</t>
+  </si>
+  <si>
+    <t>OBSERV</t>
   </si>
 </sst>
 </file>
@@ -1035,7 +1038,7 @@
   <dimension ref="A1:I23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B21"/>
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1059,7 +1062,9 @@
       <c r="E1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="4"/>
+      <c r="F1" s="4" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="2" spans="1:9">
       <c r="A2" s="2" t="s">
@@ -1284,9 +1289,13 @@
       <c r="D23" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E23" t="e">
-        <f>MEDIAN(E2:E21)</f>
-        <v>#NUM!</v>
+      <c r="E23">
+        <f>SUM(E2:E21)</f>
+        <v>0</v>
+      </c>
+      <c r="F23">
+        <f>IF(ISNUMBER(MEDIAN(F2:F21)),MEDIAN(F2:F21),0)</f>
+        <v>0</v>
       </c>
       <c r="H23" s="4"/>
       <c r="I23" s="3"/>

</xml_diff>